<commit_message>
include pTmin, pTmax in ratios
</commit_message>
<xml_diff>
--- a/proton_qT/expdata/18661.xlsx
+++ b/proton_qT/expdata/18661.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barryp/work/JAM/fitpack2/database/proton_qT/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A24C30E-05FB-E14B-9FC2-A67AD1EE56D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EF34D3-94FC-D949-9F5B-EAD3E3A95D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="4240" windowWidth="27640" windowHeight="16940" xr2:uid="{62B30F23-DD0C-AB4E-BF9F-574F6398571D}"/>
+    <workbookView xWindow="5340" yWindow="3440" windowWidth="27640" windowHeight="16940" xr2:uid="{62B30F23-DD0C-AB4E-BF9F-574F6398571D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="20">
   <si>
     <t>E</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>units</t>
+  </si>
+  <si>
+    <t>pTmin</t>
+  </si>
+  <si>
+    <t>pTmax</t>
   </si>
 </sst>
 </file>
@@ -451,15 +457,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE630C38-FFB0-E84D-B31E-BC01446DE463}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:N33"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,31 +483,37 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>800</v>
       </c>
@@ -523,32 +533,38 @@
         <v>0.25</v>
       </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
         <v>0.92900000000000005</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="I2">
-        <f>0.01*G2</f>
+      <c r="K2">
+        <f>0.01*I2</f>
         <v>9.2900000000000014E-3</v>
       </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
       <c r="L2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>800</v>
       </c>
@@ -568,32 +584,38 @@
         <v>0.75</v>
       </c>
       <c r="G3">
+        <v>0.5</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>0.94099999999999995</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I33" si="0">0.01*G3</f>
+      <c r="K3">
+        <f t="shared" ref="K3:K33" si="0">0.01*I3</f>
         <v>9.41E-3</v>
       </c>
-      <c r="J3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" t="s">
-        <v>12</v>
-      </c>
       <c r="L3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>800</v>
       </c>
@@ -612,33 +634,39 @@
       <c r="F4" s="1">
         <v>1.25</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I4">
         <v>0.95499999999999996</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>0.02</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <f t="shared" si="0"/>
         <v>9.5499999999999995E-3</v>
       </c>
-      <c r="J4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" t="s">
-        <v>12</v>
-      </c>
       <c r="L4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>800</v>
       </c>
@@ -657,33 +685,39 @@
       <c r="F5" s="1">
         <v>1.75</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2</v>
+      </c>
+      <c r="I5">
         <v>1.0269999999999999</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <f t="shared" si="0"/>
         <v>1.027E-2</v>
       </c>
-      <c r="J5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" t="s">
-        <v>12</v>
-      </c>
       <c r="L5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>800</v>
       </c>
@@ -702,33 +736,39 @@
       <c r="F6" s="1">
         <v>2.25</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="I6">
         <v>1.091</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <f t="shared" si="0"/>
         <v>1.091E-2</v>
       </c>
-      <c r="J6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" t="s">
-        <v>12</v>
-      </c>
       <c r="L6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>800</v>
       </c>
@@ -747,33 +787,39 @@
       <c r="F7" s="1">
         <v>2.75</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+      <c r="I7">
         <v>1.081</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>0.17699999999999999</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <f t="shared" si="0"/>
         <v>1.081E-2</v>
       </c>
-      <c r="J7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" t="s">
-        <v>12</v>
-      </c>
       <c r="L7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>800</v>
       </c>
@@ -792,33 +838,39 @@
       <c r="F8" s="1">
         <v>3.25</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="I8">
         <v>0.48699999999999999</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>0.122</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <f t="shared" si="0"/>
         <v>4.8700000000000002E-3</v>
       </c>
-      <c r="J8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" t="s">
-        <v>12</v>
-      </c>
       <c r="L8" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" t="s">
+        <v>16</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>800</v>
       </c>
@@ -837,33 +889,39 @@
       <c r="F9" s="1">
         <v>3.75</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4</v>
+      </c>
+      <c r="I9">
         <v>1.298</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>0.51100000000000001</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <f t="shared" si="0"/>
         <v>1.298E-2</v>
       </c>
-      <c r="J9" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" t="s">
-        <v>12</v>
-      </c>
       <c r="L9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M9" t="s">
-        <v>16</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N9" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" t="s">
+        <v>16</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>800</v>
       </c>
@@ -882,33 +940,39 @@
       <c r="F10" s="1">
         <v>4.25</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="I10">
         <v>1.1659999999999999</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>0.78500000000000003</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <f t="shared" si="0"/>
         <v>1.166E-2</v>
       </c>
-      <c r="J10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" t="s">
-        <v>12</v>
-      </c>
       <c r="L10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M10" t="s">
-        <v>16</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="N10" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" t="s">
+        <v>16</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>800</v>
       </c>
@@ -927,33 +991,39 @@
       <c r="F11">
         <v>0.25</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I11">
         <v>0.97599999999999998</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <f t="shared" si="0"/>
         <v>9.7599999999999996E-3</v>
       </c>
-      <c r="J11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" t="s">
-        <v>12</v>
-      </c>
       <c r="L11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M11" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="N11" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" t="s">
+        <v>16</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>800</v>
       </c>
@@ -972,33 +1042,39 @@
       <c r="F12">
         <v>0.75</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12">
         <v>0.96499999999999997</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>2.4E-2</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <f t="shared" si="0"/>
         <v>9.6500000000000006E-3</v>
       </c>
-      <c r="J12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" t="s">
-        <v>12</v>
-      </c>
       <c r="L12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M12" t="s">
-        <v>16</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" t="s">
+        <v>16</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>800</v>
       </c>
@@ -1017,33 +1093,39 @@
       <c r="F13" s="1">
         <v>1.25</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I13">
         <v>0.94199999999999995</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>2.7E-2</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <f t="shared" si="0"/>
         <v>9.4199999999999996E-3</v>
       </c>
-      <c r="J13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" t="s">
-        <v>12</v>
-      </c>
       <c r="L13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M13" t="s">
-        <v>16</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N13" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" t="s">
+        <v>16</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>800</v>
       </c>
@@ -1062,33 +1144,39 @@
       <c r="F14" s="1">
         <v>1.75</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2</v>
+      </c>
+      <c r="I14">
         <v>1.0269999999999999</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <f t="shared" si="0"/>
         <v>1.027E-2</v>
       </c>
-      <c r="J14" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" t="s">
-        <v>12</v>
-      </c>
       <c r="L14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M14" t="s">
-        <v>16</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N14" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" t="s">
+        <v>16</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>800</v>
       </c>
@@ -1107,33 +1195,39 @@
       <c r="F15" s="1">
         <v>2.25</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="I15">
         <v>1.0249999999999999</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <f t="shared" si="0"/>
         <v>1.0249999999999999E-2</v>
       </c>
-      <c r="J15" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" t="s">
-        <v>12</v>
-      </c>
       <c r="L15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M15" t="s">
-        <v>16</v>
-      </c>
-      <c r="N15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N15" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" t="s">
+        <v>16</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>800</v>
       </c>
@@ -1152,33 +1246,39 @@
       <c r="F16" s="1">
         <v>2.75</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H16" s="1">
+        <v>3</v>
+      </c>
+      <c r="I16">
         <v>1.204</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>0.13600000000000001</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <f t="shared" si="0"/>
         <v>1.204E-2</v>
       </c>
-      <c r="J16" t="s">
-        <v>10</v>
-      </c>
-      <c r="K16" t="s">
-        <v>12</v>
-      </c>
       <c r="L16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" t="s">
+        <v>16</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>800</v>
       </c>
@@ -1197,33 +1297,39 @@
       <c r="F17" s="1">
         <v>3.25</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
+        <v>3</v>
+      </c>
+      <c r="H17" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="I17">
         <v>1.502</v>
       </c>
-      <c r="H17">
+      <c r="J17">
         <v>0.317</v>
       </c>
-      <c r="I17">
+      <c r="K17">
         <f t="shared" si="0"/>
         <v>1.502E-2</v>
       </c>
-      <c r="J17" t="s">
-        <v>10</v>
-      </c>
-      <c r="K17" t="s">
-        <v>12</v>
-      </c>
       <c r="L17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N17" t="s">
+        <v>14</v>
+      </c>
+      <c r="O17" t="s">
+        <v>16</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>800</v>
       </c>
@@ -1242,33 +1348,39 @@
       <c r="F18" s="1">
         <v>3.75</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="H18" s="1">
+        <v>4</v>
+      </c>
+      <c r="I18">
         <v>0.91900000000000004</v>
       </c>
-      <c r="H18">
+      <c r="J18">
         <v>0.32400000000000001</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <f t="shared" si="0"/>
         <v>9.1900000000000003E-3</v>
       </c>
-      <c r="J18" t="s">
-        <v>10</v>
-      </c>
-      <c r="K18" t="s">
-        <v>12</v>
-      </c>
       <c r="L18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M18" t="s">
-        <v>16</v>
-      </c>
-      <c r="N18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="N18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" t="s">
+        <v>16</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>800</v>
       </c>
@@ -1287,33 +1399,39 @@
       <c r="F19">
         <v>0.25</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I19">
         <v>0.89400000000000002</v>
       </c>
-      <c r="H19">
+      <c r="J19">
         <v>0.05</v>
       </c>
-      <c r="I19">
+      <c r="K19">
         <f t="shared" si="0"/>
         <v>8.94E-3</v>
       </c>
-      <c r="J19" t="s">
-        <v>10</v>
-      </c>
-      <c r="K19" t="s">
-        <v>12</v>
-      </c>
       <c r="L19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M19" t="s">
-        <v>16</v>
-      </c>
-      <c r="N19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="N19" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" t="s">
+        <v>16</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>800</v>
       </c>
@@ -1332,33 +1450,39 @@
       <c r="F20">
         <v>0.75</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20">
         <v>0.88700000000000001</v>
       </c>
-      <c r="H20">
+      <c r="J20">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="I20">
+      <c r="K20">
         <f t="shared" si="0"/>
         <v>8.8700000000000011E-3</v>
       </c>
-      <c r="J20" t="s">
-        <v>10</v>
-      </c>
-      <c r="K20" t="s">
-        <v>12</v>
-      </c>
       <c r="L20" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M20" t="s">
-        <v>16</v>
-      </c>
-      <c r="N20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N20" t="s">
+        <v>14</v>
+      </c>
+      <c r="O20" t="s">
+        <v>16</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>800</v>
       </c>
@@ -1377,33 +1501,39 @@
       <c r="F21" s="1">
         <v>1.25</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I21">
         <v>1.08</v>
       </c>
-      <c r="H21">
+      <c r="J21">
         <v>0.05</v>
       </c>
-      <c r="I21">
+      <c r="K21">
         <f t="shared" si="0"/>
         <v>1.0800000000000001E-2</v>
       </c>
-      <c r="J21" t="s">
-        <v>10</v>
-      </c>
-      <c r="K21" t="s">
-        <v>12</v>
-      </c>
       <c r="L21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M21" t="s">
-        <v>16</v>
-      </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O21" t="s">
+        <v>16</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>800</v>
       </c>
@@ -1422,33 +1552,39 @@
       <c r="F22" s="1">
         <v>1.75</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="H22" s="1">
+        <v>2</v>
+      </c>
+      <c r="I22">
         <v>1.0620000000000001</v>
       </c>
-      <c r="H22">
+      <c r="J22">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="I22">
+      <c r="K22">
         <f t="shared" si="0"/>
         <v>1.0620000000000001E-2</v>
       </c>
-      <c r="J22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22" t="s">
-        <v>12</v>
-      </c>
       <c r="L22" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M22" t="s">
-        <v>16</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N22" t="s">
+        <v>14</v>
+      </c>
+      <c r="O22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>800</v>
       </c>
@@ -1467,33 +1603,39 @@
       <c r="F23" s="1">
         <v>2.25</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="1">
+        <v>2</v>
+      </c>
+      <c r="H23" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="I23">
         <v>1.008</v>
       </c>
-      <c r="H23">
+      <c r="J23">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="I23">
+      <c r="K23">
         <f t="shared" si="0"/>
         <v>1.008E-2</v>
       </c>
-      <c r="J23" t="s">
-        <v>10</v>
-      </c>
-      <c r="K23" t="s">
-        <v>12</v>
-      </c>
       <c r="L23" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M23" t="s">
-        <v>16</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N23" t="s">
+        <v>14</v>
+      </c>
+      <c r="O23" t="s">
+        <v>16</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>800</v>
       </c>
@@ -1512,33 +1654,39 @@
       <c r="F24" s="1">
         <v>2.75</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3</v>
+      </c>
+      <c r="I24">
         <v>1.2010000000000001</v>
       </c>
-      <c r="H24">
+      <c r="J24">
         <v>0.21299999999999999</v>
       </c>
-      <c r="I24">
+      <c r="K24">
         <f t="shared" si="0"/>
         <v>1.2010000000000002E-2</v>
       </c>
-      <c r="J24" t="s">
-        <v>10</v>
-      </c>
-      <c r="K24" t="s">
-        <v>12</v>
-      </c>
       <c r="L24" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M24" t="s">
-        <v>16</v>
-      </c>
-      <c r="N24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N24" t="s">
+        <v>14</v>
+      </c>
+      <c r="O24" t="s">
+        <v>16</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>800</v>
       </c>
@@ -1557,33 +1705,39 @@
       <c r="F25" s="1">
         <v>3.25</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
+        <v>3</v>
+      </c>
+      <c r="H25" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="I25">
         <v>1.0720000000000001</v>
       </c>
-      <c r="H25">
+      <c r="J25">
         <v>0.25700000000000001</v>
       </c>
-      <c r="I25">
+      <c r="K25">
         <f t="shared" si="0"/>
         <v>1.072E-2</v>
       </c>
-      <c r="J25" t="s">
-        <v>10</v>
-      </c>
-      <c r="K25" t="s">
-        <v>12</v>
-      </c>
       <c r="L25" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M25" t="s">
-        <v>16</v>
-      </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N25" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" t="s">
+        <v>16</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>800</v>
       </c>
@@ -1602,33 +1756,39 @@
       <c r="F26" s="1">
         <v>3.75</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="H26" s="1">
+        <v>4</v>
+      </c>
+      <c r="I26">
         <v>0.98199999999999998</v>
       </c>
-      <c r="H26">
+      <c r="J26">
         <v>0.40400000000000003</v>
       </c>
-      <c r="I26">
+      <c r="K26">
         <f t="shared" si="0"/>
         <v>9.8200000000000006E-3</v>
       </c>
-      <c r="J26" t="s">
-        <v>10</v>
-      </c>
-      <c r="K26" t="s">
-        <v>12</v>
-      </c>
       <c r="L26" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="N26" t="s">
+        <v>14</v>
+      </c>
+      <c r="O26" t="s">
+        <v>16</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>800</v>
       </c>
@@ -1647,33 +1807,39 @@
       <c r="F27">
         <v>0.25</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I27">
         <v>0.98599999999999999</v>
       </c>
-      <c r="H27">
+      <c r="J27">
         <v>0.113</v>
       </c>
-      <c r="I27">
+      <c r="K27">
         <f t="shared" si="0"/>
         <v>9.8600000000000007E-3</v>
       </c>
-      <c r="J27" t="s">
-        <v>10</v>
-      </c>
-      <c r="K27" t="s">
-        <v>12</v>
-      </c>
       <c r="L27" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M27" t="s">
-        <v>16</v>
-      </c>
-      <c r="N27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="N27" t="s">
+        <v>14</v>
+      </c>
+      <c r="O27" t="s">
+        <v>16</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>800</v>
       </c>
@@ -1692,33 +1858,39 @@
       <c r="F28">
         <v>0.75</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28">
         <v>0.98</v>
       </c>
-      <c r="H28">
+      <c r="J28">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="I28">
+      <c r="K28">
         <f t="shared" si="0"/>
         <v>9.7999999999999997E-3</v>
       </c>
-      <c r="J28" t="s">
-        <v>10</v>
-      </c>
-      <c r="K28" t="s">
-        <v>12</v>
-      </c>
       <c r="L28" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M28" t="s">
-        <v>16</v>
-      </c>
-      <c r="N28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O28" t="s">
+        <v>16</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>800</v>
       </c>
@@ -1737,33 +1909,39 @@
       <c r="F29" s="1">
         <v>1.25</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I29">
         <v>1.0569999999999999</v>
       </c>
-      <c r="H29">
+      <c r="J29">
         <v>0.08</v>
       </c>
-      <c r="I29">
+      <c r="K29">
         <f t="shared" si="0"/>
         <v>1.057E-2</v>
       </c>
-      <c r="J29" t="s">
-        <v>10</v>
-      </c>
-      <c r="K29" t="s">
-        <v>12</v>
-      </c>
       <c r="L29" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M29" t="s">
-        <v>16</v>
-      </c>
-      <c r="N29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N29" t="s">
+        <v>14</v>
+      </c>
+      <c r="O29" t="s">
+        <v>16</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>800</v>
       </c>
@@ -1782,33 +1960,39 @@
       <c r="F30" s="1">
         <v>1.75</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="H30" s="1">
+        <v>2</v>
+      </c>
+      <c r="I30">
         <v>1.0249999999999999</v>
       </c>
-      <c r="H30">
+      <c r="J30">
         <v>0.108</v>
       </c>
-      <c r="I30">
+      <c r="K30">
         <f t="shared" si="0"/>
         <v>1.0249999999999999E-2</v>
       </c>
-      <c r="J30" t="s">
-        <v>10</v>
-      </c>
-      <c r="K30" t="s">
-        <v>12</v>
-      </c>
       <c r="L30" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M30" t="s">
-        <v>16</v>
-      </c>
-      <c r="N30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N30" t="s">
+        <v>14</v>
+      </c>
+      <c r="O30" t="s">
+        <v>16</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>800</v>
       </c>
@@ -1827,33 +2011,39 @@
       <c r="F31" s="1">
         <v>2.25</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="1">
+        <v>2</v>
+      </c>
+      <c r="H31" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="I31">
         <v>1.1519999999999999</v>
       </c>
-      <c r="H31">
+      <c r="J31">
         <v>0.184</v>
       </c>
-      <c r="I31">
+      <c r="K31">
         <f t="shared" si="0"/>
         <v>1.1519999999999999E-2</v>
       </c>
-      <c r="J31" t="s">
-        <v>10</v>
-      </c>
-      <c r="K31" t="s">
-        <v>12</v>
-      </c>
       <c r="L31" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M31" t="s">
-        <v>16</v>
-      </c>
-      <c r="N31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N31" t="s">
+        <v>14</v>
+      </c>
+      <c r="O31" t="s">
+        <v>16</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>800</v>
       </c>
@@ -1872,33 +2062,39 @@
       <c r="F32" s="1">
         <v>2.75</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H32" s="1">
+        <v>3</v>
+      </c>
+      <c r="I32">
         <v>1.0649999999999999</v>
       </c>
-      <c r="H32">
+      <c r="J32">
         <v>0.254</v>
       </c>
-      <c r="I32">
+      <c r="K32">
         <f t="shared" si="0"/>
         <v>1.065E-2</v>
       </c>
-      <c r="J32" t="s">
-        <v>10</v>
-      </c>
-      <c r="K32" t="s">
-        <v>12</v>
-      </c>
       <c r="L32" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M32" t="s">
-        <v>16</v>
-      </c>
-      <c r="N32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="N32" t="s">
+        <v>14</v>
+      </c>
+      <c r="O32" t="s">
+        <v>16</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>800</v>
       </c>
@@ -1917,29 +2113,35 @@
       <c r="F33" s="1">
         <v>3.25</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
+        <v>3</v>
+      </c>
+      <c r="H33" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="I33">
         <v>0.94499999999999995</v>
       </c>
-      <c r="H33">
+      <c r="J33">
         <v>0.60799999999999998</v>
       </c>
-      <c r="I33">
+      <c r="K33">
         <f t="shared" si="0"/>
         <v>9.4500000000000001E-3</v>
       </c>
-      <c r="J33" t="s">
-        <v>10</v>
-      </c>
-      <c r="K33" t="s">
-        <v>12</v>
-      </c>
       <c r="L33" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="M33" t="s">
-        <v>16</v>
-      </c>
-      <c r="N33">
+        <v>12</v>
+      </c>
+      <c r="N33" t="s">
+        <v>14</v>
+      </c>
+      <c r="O33" t="s">
+        <v>16</v>
+      </c>
+      <c r="P33">
         <v>1</v>
       </c>
     </row>

</xml_diff>